<commit_message>
update code to create cctb sense table, and include tables
</commit_message>
<xml_diff>
--- a/fixme/shifters_move_labels.xlsx
+++ b/fixme/shifters_move_labels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afern\Documents\UMD\LHCb\cern\LV_cavern_mapping\fixme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AD211D4C-E7F8-45D8-976C-A2E81CD18CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BAE276-61C0-40BA-A1A7-093BEEB2F607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-19350" yWindow="-4460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="move_labels" sheetId="1" r:id="rId1"/>
@@ -1423,7 +1423,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1583,7 +1583,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1763,6 +1763,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1933,7 +1939,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1951,6 +1957,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2307,11 +2316,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" topLeftCell="K150" workbookViewId="0">
+      <selection activeCell="L165" sqref="L165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3313,7 +3322,7 @@
       <c r="K26" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="L26" s="4" t="s">
+      <c r="L26" s="7" t="s">
         <v>103</v>
       </c>
     </row>
@@ -4149,7 +4158,7 @@
       <c r="K48" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="L48" s="4" t="s">
+      <c r="L48" s="7" t="s">
         <v>169</v>
       </c>
     </row>
@@ -4947,7 +4956,7 @@
       <c r="K69" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="L69" s="4" t="s">
+      <c r="L69" s="7" t="s">
         <v>232</v>
       </c>
     </row>
@@ -8101,7 +8110,7 @@
       <c r="K152" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="L152" s="4" t="s">
+      <c r="L152" s="7" t="s">
         <v>102</v>
       </c>
     </row>
@@ -8329,7 +8338,7 @@
       <c r="K158" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="L158" s="4" t="s">
+      <c r="L158" s="7" t="s">
         <v>168</v>
       </c>
     </row>
@@ -8519,7 +8528,7 @@
       <c r="K163" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="L163" s="4" t="s">
+      <c r="L163" s="7" t="s">
         <v>193</v>
       </c>
     </row>

</xml_diff>